<commit_message>
start to calculate end date
</commit_message>
<xml_diff>
--- a/burnupreporting/TrackingAProjectASL.xlsx
+++ b/burnupreporting/TrackingAProjectASL.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marks\Documents\GitHub\asl-reporting\burnupreporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80511272-3931-40B1-B1CC-6DB585D1F5ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A299ADFC-53ED-4431-93B1-479F3B5AF90C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="15390" windowHeight="7170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="15390" windowHeight="7170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
-    <sheet name="burnup data" sheetId="11" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="14" r:id="rId3"/>
-    <sheet name="Dashboard" sheetId="12" r:id="rId4"/>
+    <sheet name="burnup chart" sheetId="15" r:id="rId2"/>
+    <sheet name="burnup data" sheetId="11" r:id="rId3"/>
+    <sheet name="dashboard" sheetId="12" r:id="rId4"/>
     <sheet name="assessors questions" sheetId="7" state="hidden" r:id="rId5"/>
     <sheet name="reporting audit" sheetId="8" state="hidden" r:id="rId6"/>
   </sheets>
@@ -27,7 +27,6 @@
     <definedName name="total">data!$F$15</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
   <si>
     <t>project</t>
   </si>
@@ -264,10 +263,16 @@
     <t>Actual Total Velocity</t>
   </si>
   <si>
-    <t>Burn</t>
-  </si>
-  <si>
     <t>Total Work</t>
+  </si>
+  <si>
+    <t>Current date</t>
+  </si>
+  <si>
+    <t>Current Sprint</t>
+  </si>
+  <si>
+    <t>Likely date of completion</t>
   </si>
 </sst>
 </file>
@@ -344,7 +349,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -376,6 +381,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -410,6 +416,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>ASL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Burnup Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -672,7 +708,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E9DA-4F05-855A-79476F6821AD}"/>
+              <c16:uniqueId val="{00000000-BC03-46B2-A53D-E48635E93F79}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -903,7 +939,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E9DA-4F05-855A-79476F6821AD}"/>
+              <c16:uniqueId val="{00000001-BC03-46B2-A53D-E48635E93F79}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -957,7 +993,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1052,6 +1088,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.54197993888826856"/>
+          <c:y val="0.69548142618732511"/>
+          <c:w val="0.30867053836832969"/>
+          <c:h val="3.4059869938891714E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1110,11 +1156,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1674,31 +1715,34 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A42B397C-E8E9-421D-BD38-13E5090ED0D1}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1025525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>244475</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668712" cy="6292273"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E07B7276-1FE0-4A2B-B4C5-9C41C3E62262}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EB85CF-A52A-477E-95E0-A26A6415B40B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1711,7 +1755,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2004,7 +2048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -5584,32 +5628,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0428A0C-7D92-48CE-8174-3FCE0A91D90D}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="12" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
     <col min="5" max="5" width="16.6328125" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" customWidth="1"/>
+    <col min="6" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="28.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>70</v>
@@ -5620,11 +5664,11 @@
       <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>43222</v>
       </c>
@@ -5644,11 +5688,15 @@
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" s="12">
+        <f>A2</f>
+        <v>43222</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <f>A2+14</f>
         <v>43236</v>
@@ -5667,10 +5715,14 @@
         <f>F2+D3</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="12">
+        <f t="shared" ref="G3:G29" si="0">A3</f>
+        <v>43236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
-        <f t="shared" ref="A4:A45" si="0">A3+14</f>
+        <f t="shared" ref="A4:A29" si="1">A3+14</f>
         <v>43250</v>
       </c>
       <c r="B4">
@@ -5684,13 +5736,17 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F10" si="1">F3+D4</f>
+        <f t="shared" ref="F4:F10" si="2">F3+D4</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43264</v>
       </c>
       <c r="B5">
@@ -5704,13 +5760,17 @@
         <v>6</v>
       </c>
       <c r="F5">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>43264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
         <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="12">
-        <f t="shared" si="0"/>
         <v>43278</v>
       </c>
       <c r="B6">
@@ -5724,13 +5784,17 @@
         <v>6</v>
       </c>
       <c r="F6">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="0"/>
+        <v>43278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
-        <f t="shared" si="0"/>
         <v>43292</v>
       </c>
       <c r="B7">
@@ -5744,13 +5808,17 @@
         <v>6</v>
       </c>
       <c r="F7">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="0"/>
+        <v>43292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
-        <f t="shared" si="0"/>
         <v>43306</v>
       </c>
       <c r="B8">
@@ -5764,13 +5832,17 @@
         <v>6</v>
       </c>
       <c r="F8">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="0"/>
+        <v>43306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
         <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="12">
-        <f t="shared" si="0"/>
         <v>43320</v>
       </c>
       <c r="B9">
@@ -5784,13 +5856,17 @@
         <v>6</v>
       </c>
       <c r="F9">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="0"/>
+        <v>43320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="12">
-        <f t="shared" si="0"/>
         <v>43334</v>
       </c>
       <c r="B10">
@@ -5804,13 +5880,17 @@
         <v>6</v>
       </c>
       <c r="F10">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="0"/>
+        <v>43334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
         <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="12">
-        <f t="shared" si="0"/>
         <v>43348</v>
       </c>
       <c r="B11">
@@ -5824,13 +5904,17 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F20" si="2">F10+D11</f>
+        <f t="shared" ref="F11:F20" si="3">F10+D11</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" s="12">
+        <f t="shared" si="0"/>
+        <v>43348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43362</v>
       </c>
       <c r="B12">
@@ -5844,13 +5928,17 @@
         <v>6</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G12" s="12">
+        <f t="shared" si="0"/>
+        <v>43362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43376</v>
       </c>
       <c r="B13">
@@ -5864,13 +5952,17 @@
         <v>6</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" s="12">
+        <f t="shared" si="0"/>
+        <v>43376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43390</v>
       </c>
       <c r="B14">
@@ -5884,13 +5976,17 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" s="12">
+        <f t="shared" si="0"/>
+        <v>43390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43404</v>
       </c>
       <c r="B15">
@@ -5904,13 +6000,17 @@
         <v>6</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="12">
+        <f t="shared" si="0"/>
+        <v>43404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43418</v>
       </c>
       <c r="B16">
@@ -5924,13 +6024,17 @@
         <v>6</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="12">
+        <f t="shared" si="0"/>
+        <v>43418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43432</v>
       </c>
       <c r="B17">
@@ -5944,13 +6048,17 @@
         <v>6</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="12">
+        <f t="shared" si="0"/>
+        <v>43432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43446</v>
       </c>
       <c r="B18">
@@ -5964,13 +6072,17 @@
         <v>6</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="12">
+        <f t="shared" si="0"/>
+        <v>43446</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43460</v>
       </c>
       <c r="B19">
@@ -5984,13 +6096,17 @@
         <v>6</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="12">
+        <f t="shared" si="0"/>
+        <v>43460</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43474</v>
       </c>
       <c r="B20">
@@ -6004,13 +6120,17 @@
         <v>6</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="12">
+        <f t="shared" si="0"/>
+        <v>43474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43488</v>
       </c>
       <c r="B21">
@@ -6024,13 +6144,17 @@
         <v>6</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F45" si="3">F20+D21</f>
+        <f t="shared" ref="F21:F29" si="4">F20+D21</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="12">
+        <f t="shared" si="0"/>
+        <v>43488</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43502</v>
       </c>
       <c r="B22">
@@ -6044,13 +6168,17 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="12">
+        <f t="shared" si="0"/>
+        <v>43502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43516</v>
       </c>
       <c r="B23">
@@ -6064,13 +6192,17 @@
         <v>6</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="12">
+        <f t="shared" si="0"/>
+        <v>43516</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43530</v>
       </c>
       <c r="B24">
@@ -6084,13 +6216,17 @@
         <v>6</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="12">
+        <f t="shared" si="0"/>
+        <v>43530</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43544</v>
       </c>
       <c r="B25">
@@ -6104,13 +6240,17 @@
         <v>6</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="12">
+        <f t="shared" si="0"/>
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43558</v>
       </c>
       <c r="B26">
@@ -6124,13 +6264,17 @@
         <v>6</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="12">
+        <f t="shared" si="0"/>
+        <v>43558</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43572</v>
       </c>
       <c r="B27">
@@ -6144,13 +6288,17 @@
         <v>6</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="12">
+        <f t="shared" si="0"/>
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43586</v>
       </c>
       <c r="B28">
@@ -6164,13 +6312,17 @@
         <v>6</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>162</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="12">
+        <f t="shared" si="0"/>
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43600</v>
       </c>
       <c r="B29">
@@ -6184,75 +6336,58 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
+      <c r="G29" s="12">
+        <f t="shared" si="0"/>
+        <v>43600</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EAAA29-82D1-4D73-943E-31FED8BFB5CC}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE32384-8F99-4706-944C-3810A822F9CF}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B1" s="12">
+        <f ca="1">TODAY()</f>
+        <v>43213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="13">
+        <f ca="1">ROUND(('burnup data'!A2-TODAY())/14+'burnup data'!B2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="12">
+        <f>VLOOKUP(total,'burnup data'!F2:G29,2)</f>
+        <v>43586</v>
       </c>
     </row>
   </sheetData>
@@ -6261,18 +6396,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE32384-8F99-4706-944C-3810A822F9CF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -6340,7 +6463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -6673,20 +6796,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="5663049d-d602-4310-a81b-99d4dd01da5c">
-      <UserInfo>
-        <DisplayName>Home Office Digital</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008AFD548CC043154FB6083CDAD62397B4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cb13562aef696428004616f280f0c63c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5663049d-d602-4310-a81b-99d4dd01da5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f72fef54cac438e4c919ed53a805a4b1" ns2:_="">
     <xsd:import namespace="5663049d-d602-4310-a81b-99d4dd01da5c"/>
@@ -6834,6 +6943,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="5663049d-d602-4310-a81b-99d4dd01da5c">
+      <UserInfo>
+        <DisplayName>Home Office Digital</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB969E2F-BEC8-4539-AA2C-F9E82E7EFF8F}">
   <ds:schemaRefs>
@@ -6843,22 +6966,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F5DB09-79F3-4A55-8F8C-672DEE497621}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5663049d-d602-4310-a81b-99d4dd01da5c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA52E8BC-B844-4707-BB0D-8F006DA6E8B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6874,4 +6981,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F5DB09-79F3-4A55-8F8C-672DEE497621}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5663049d-d602-4310-a81b-99d4dd01da5c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>